<commit_message>
Medição da Sprint 6 realizada
</commit_message>
<xml_diff>
--- a/docs/project/STE_GQ_Checklists/STE_CA_ChecklistDeAvaliacao_Sprint-06.xlsx
+++ b/docs/project/STE_GQ_Checklists/STE_CA_ChecklistDeAvaliacao_Sprint-06.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GRE" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="NECESSITA_MUDANÇAS" comment="Lista Suspensa de STATUS">#REF!</definedName>
     <definedName name="NomeGerenteQualidade">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -177,6 +177,24 @@
   </si>
   <si>
     <t>Sprint: 6</t>
+  </si>
+  <si>
+    <t>Riscos não foram atualizados</t>
+  </si>
+  <si>
+    <t>Cronograma não foi definido</t>
+  </si>
+  <si>
+    <t>Lições aprendidas não foram registradas</t>
+  </si>
+  <si>
+    <t>Houve atraso nas revisões</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existem problemas de padronização </t>
+  </si>
+  <si>
+    <t>Não foram executadas correções de código</t>
   </si>
 </sst>
 </file>
@@ -358,7 +376,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,6 +427,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Euro" xfId="2"/>
@@ -946,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1114,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1191,14 +1212,14 @@
         <v>13</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4" t="str">
         <f>IF(C5=0,"Estável",IF(C5&lt;=3,"Necessita de Atenção","Necessita de Mudança"))</f>
-        <v>Estável</v>
+        <v>Necessita de Atenção</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1227,14 +1248,14 @@
         <v>14</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Estável</v>
+        <v>Necessita de Atenção</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1281,14 +1302,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Estável</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
+        <v>Necessita de Atenção</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1335,14 +1356,14 @@
         <v>25</v>
       </c>
       <c r="C13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Estável</v>
+        <v>Necessita de Atenção</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,7 +1372,7 @@
       </c>
       <c r="C15" s="13">
         <f>SUM(C4:C13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1699,14 +1720,14 @@
         <v>34</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>736</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Estável</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>43</v>
+        <v>Necessita de Mudança</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1735,14 +1756,14 @@
         <v>35</v>
       </c>
       <c r="C9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Estável</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>Necessita de Atenção</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +1772,7 @@
       </c>
       <c r="C11" s="13">
         <f>SUM(C4:C9)</f>
-        <v>0</v>
+        <v>737</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1792,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>